<commit_message>
Added more detail to ARMA models, correct errors in variable naming of AR and MA processes
</commit_message>
<xml_diff>
--- a/Project2/Data/winedata.xlsx
+++ b/Project2/Data/winedata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/087f5d83ccd9606c/Desktop/GitRepos/Deeplearning-Workshops-FYP/Project2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC10489919D95FBE5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69E3985C-9C7A-46B0-8F9F-CEBCB30A209A}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABDACC10489919D95FBE5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FA392B8-6E0D-472A-AC50-3759AE2637B6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,6 +81,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,7 +353,7 @@
   <dimension ref="A1:A143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A143"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>